<commit_message>
edited shredding yield and al content
</commit_message>
<xml_diff>
--- a/data/Collection.xlsx
+++ b/data/Collection.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\romainb\Documents\6. Papers\6. Dynamic MFA Al in Passenger cars\model with segments and powertrain\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\home.ansatt.ntnu.no\romainb\Documents\6. Papers\6. Dynamic MFA Al in Passenger cars\Dynamic-MFA-Al-in-Passenger-Cars\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14EC7E1B-14E2-4C3F-BEA3-1CDD00DFC4B3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FEE9F32-26F6-484F-8C90-5D9433020B7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{66C38FE6-7F1B-4F07-9DE9-E34F60D40B66}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{66C38FE6-7F1B-4F07-9DE9-E34F60D40B66}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="2" r:id="rId1"/>
     <sheet name="Data" sheetId="1" r:id="rId2"/>
-    <sheet name="Sheet1" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029" iterate="1" iterateCount="1000"/>
   <extLst>
@@ -142,9 +141,6 @@
     <t>Last modified by</t>
   </si>
   <si>
-    <t>Pristera</t>
-  </si>
-  <si>
     <t># Name of researcher responsible for last modification</t>
   </si>
   <si>
@@ -242,6 +238,9 @@
   </si>
   <si>
     <t>ODYM_Classifications_Master_Al_cars</t>
+  </si>
+  <si>
+    <t>Romain Billy</t>
   </si>
 </sst>
 </file>
@@ -661,19 +660,19 @@
   <dimension ref="A1:H28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="34.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="38.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.6640625" customWidth="1"/>
-    <col min="4" max="4" width="17.88671875" customWidth="1"/>
+    <col min="1" max="1" width="34.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="38.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" customWidth="1"/>
+    <col min="4" max="4" width="17.85546875" customWidth="1"/>
     <col min="6" max="6" width="18" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
@@ -691,7 +690,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>4</v>
       </c>
@@ -711,12 +710,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>7</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
@@ -729,12 +728,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>9</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>10</v>
@@ -751,7 +750,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>13</v>
       </c>
@@ -773,7 +772,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>16</v>
       </c>
@@ -795,7 +794,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>19</v>
       </c>
@@ -815,7 +814,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>23</v>
       </c>
@@ -833,12 +832,12 @@
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>26</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
@@ -851,12 +850,12 @@
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>28</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
@@ -869,7 +868,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>30</v>
       </c>
@@ -887,12 +886,12 @@
         <v>31</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>32</v>
       </c>
       <c r="B12" s="10">
-        <v>43977</v>
+        <v>44802</v>
       </c>
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
@@ -905,12 +904,12 @@
         <v>33</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>34</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>35</v>
+        <v>68</v>
       </c>
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
@@ -920,15 +919,15 @@
         <v>2</v>
       </c>
       <c r="H13" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A14" s="5" t="s">
+      <c r="B14" s="8" t="s">
         <v>37</v>
-      </c>
-      <c r="B14" s="8" t="s">
-        <v>38</v>
       </c>
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
@@ -938,15 +937,15 @@
         <v>2</v>
       </c>
       <c r="H14" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="5" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A15" s="5" t="s">
-        <v>40</v>
-      </c>
       <c r="B15" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
@@ -956,12 +955,12 @@
         <v>2</v>
       </c>
       <c r="H15" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
         <v>41</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A16" s="1" t="s">
-        <v>42</v>
       </c>
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
@@ -971,9 +970,9 @@
       <c r="G16" s="4"/>
       <c r="H16" s="3"/>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
@@ -983,9 +982,9 @@
       <c r="G17" s="4"/>
       <c r="H17" s="3"/>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
@@ -995,9 +994,9 @@
       <c r="G18" s="4"/>
       <c r="H18" s="3"/>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
@@ -1007,9 +1006,9 @@
       <c r="G19" s="4"/>
       <c r="H19" s="3"/>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
@@ -1019,21 +1018,21 @@
       <c r="G20" s="4"/>
       <c r="H20" s="3"/>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>20</v>
       </c>
       <c r="C21" s="11" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D21" s="12">
         <v>151</v>
       </c>
       <c r="E21" s="11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F21" s="12">
         <v>5</v>
@@ -1042,60 +1041,60 @@
         <v>2</v>
       </c>
       <c r="H21" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" s="5" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A22" s="5" t="s">
+      <c r="B22" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="B22" s="5" t="s">
+      <c r="C22" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="C22" s="5" t="s">
+      <c r="D22" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="D22" s="5" t="s">
+      <c r="E22" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="E22" s="5" t="s">
+      <c r="F22" s="5" t="s">
         <v>51</v>
-      </c>
-      <c r="F22" s="5" t="s">
-        <v>52</v>
       </c>
       <c r="G22" s="4" t="s">
         <v>2</v>
       </c>
       <c r="H22" s="3"/>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C23" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="D23" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="D23" s="3" t="s">
+      <c r="E23" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="E23" s="8" t="s">
-        <v>55</v>
-      </c>
       <c r="F23" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G23" s="4" t="s">
         <v>2</v>
       </c>
       <c r="H23" s="3" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E24" s="4" t="s">
         <v>2</v>
       </c>
@@ -1106,10 +1105,10 @@
         <v>2</v>
       </c>
       <c r="H24" s="3" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D25" s="3"/>
       <c r="E25" s="3"/>
       <c r="F25" s="3"/>
@@ -1117,20 +1116,20 @@
         <v>2</v>
       </c>
       <c r="H25" s="3" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E26" s="3"/>
       <c r="F26" s="3"/>
       <c r="G26" s="4" t="s">
         <v>2</v>
       </c>
       <c r="H26" s="3" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E27" s="3"/>
       <c r="F27" s="3"/>
       <c r="G27" s="4" t="s">
@@ -1138,7 +1137,7 @@
       </c>
       <c r="H27" s="3"/>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="3"/>
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
@@ -1150,6 +1149,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1157,36 +1157,36 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F525485-5BF7-4B7F-9D80-F8AD30318E4F}">
   <dimension ref="A1:F152"/>
   <sheetViews>
-    <sheetView topLeftCell="A97" workbookViewId="0">
+    <sheetView topLeftCell="A79" workbookViewId="0">
       <selection activeCell="I120" sqref="I120"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.109375" style="1"/>
+    <col min="1" max="1" width="9.140625" style="1"/>
     <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1900</v>
       </c>
@@ -1208,7 +1208,7 @@
         <v>0.38945000000000363</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1901</v>
       </c>
@@ -1230,7 +1230,7 @@
         <v>0.38945000000000363</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>1902</v>
       </c>
@@ -1252,7 +1252,7 @@
         <v>0.38945000000000363</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>1903</v>
       </c>
@@ -1274,7 +1274,7 @@
         <v>0.38945000000000363</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>1904</v>
       </c>
@@ -1296,7 +1296,7 @@
         <v>0.38945000000000363</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>1905</v>
       </c>
@@ -1318,7 +1318,7 @@
         <v>0.38945000000000363</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>1906</v>
       </c>
@@ -1340,7 +1340,7 @@
         <v>0.38945000000000363</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>1907</v>
       </c>
@@ -1362,7 +1362,7 @@
         <v>0.38945000000000363</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>1908</v>
       </c>
@@ -1384,7 +1384,7 @@
         <v>0.38945000000000363</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>1909</v>
       </c>
@@ -1406,7 +1406,7 @@
         <v>0.38945000000000363</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>1910</v>
       </c>
@@ -1428,7 +1428,7 @@
         <v>0.38945000000000363</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>1911</v>
       </c>
@@ -1450,7 +1450,7 @@
         <v>0.38945000000000363</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>1912</v>
       </c>
@@ -1472,7 +1472,7 @@
         <v>0.38945000000000363</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>1913</v>
       </c>
@@ -1494,7 +1494,7 @@
         <v>0.38945000000000363</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>1914</v>
       </c>
@@ -1516,7 +1516,7 @@
         <v>0.38945000000000363</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>1915</v>
       </c>
@@ -1538,7 +1538,7 @@
         <v>0.38945000000000363</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>1916</v>
       </c>
@@ -1560,7 +1560,7 @@
         <v>0.38945000000000363</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>1917</v>
       </c>
@@ -1582,7 +1582,7 @@
         <v>0.38945000000000363</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>1918</v>
       </c>
@@ -1604,7 +1604,7 @@
         <v>0.38945000000000363</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>1919</v>
       </c>
@@ -1626,7 +1626,7 @@
         <v>0.38945000000000363</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>1920</v>
       </c>
@@ -1648,7 +1648,7 @@
         <v>0.38945000000000363</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>1921</v>
       </c>
@@ -1670,7 +1670,7 @@
         <v>0.38945000000000363</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>1922</v>
       </c>
@@ -1692,7 +1692,7 @@
         <v>0.38945000000000363</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>1923</v>
       </c>
@@ -1714,7 +1714,7 @@
         <v>0.38945000000000363</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>1924</v>
       </c>
@@ -1736,7 +1736,7 @@
         <v>0.38945000000000363</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>1925</v>
       </c>
@@ -1758,7 +1758,7 @@
         <v>0.38945000000000363</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>1926</v>
       </c>
@@ -1780,7 +1780,7 @@
         <v>0.38945000000000363</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>1927</v>
       </c>
@@ -1802,7 +1802,7 @@
         <v>0.38945000000000363</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>1928</v>
       </c>
@@ -1824,7 +1824,7 @@
         <v>0.38945000000000363</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>1929</v>
       </c>
@@ -1846,7 +1846,7 @@
         <v>0.38945000000000363</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>1930</v>
       </c>
@@ -1868,7 +1868,7 @@
         <v>0.38945000000000363</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>1931</v>
       </c>
@@ -1890,7 +1890,7 @@
         <v>0.38945000000000363</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>1932</v>
       </c>
@@ -1912,7 +1912,7 @@
         <v>0.38945000000000363</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>1933</v>
       </c>
@@ -1934,7 +1934,7 @@
         <v>0.38945000000000363</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>1934</v>
       </c>
@@ -1956,7 +1956,7 @@
         <v>0.38945000000000363</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>1935</v>
       </c>
@@ -1978,7 +1978,7 @@
         <v>0.38945000000000363</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>1936</v>
       </c>
@@ -2000,7 +2000,7 @@
         <v>0.38945000000000363</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>1937</v>
       </c>
@@ -2022,7 +2022,7 @@
         <v>0.38945000000000363</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>1938</v>
       </c>
@@ -2044,7 +2044,7 @@
         <v>0.38945000000000363</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>1939</v>
       </c>
@@ -2066,7 +2066,7 @@
         <v>0.38945000000000363</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>1940</v>
       </c>
@@ -2088,7 +2088,7 @@
         <v>0.38945000000000363</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>1941</v>
       </c>
@@ -2110,7 +2110,7 @@
         <v>0.38945000000000363</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>1942</v>
       </c>
@@ -2132,7 +2132,7 @@
         <v>0.38945000000000363</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>1943</v>
       </c>
@@ -2154,7 +2154,7 @@
         <v>0.38945000000000363</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>1944</v>
       </c>
@@ -2176,7 +2176,7 @@
         <v>0.38945000000000363</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>1945</v>
       </c>
@@ -2198,7 +2198,7 @@
         <v>0.38945000000000363</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>1946</v>
       </c>
@@ -2220,7 +2220,7 @@
         <v>0.38945000000000363</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>1947</v>
       </c>
@@ -2242,7 +2242,7 @@
         <v>0.38945000000000363</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>1948</v>
       </c>
@@ -2264,7 +2264,7 @@
         <v>0.38945000000000363</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <v>1949</v>
       </c>
@@ -2286,7 +2286,7 @@
         <v>0.38945000000000363</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <v>1950</v>
       </c>
@@ -2307,7 +2307,7 @@
         <v>0.38945000000000363</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <v>1951</v>
       </c>
@@ -2328,7 +2328,7 @@
         <v>0.41056100000000129</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <v>1952</v>
       </c>
@@ -2349,7 +2349,7 @@
         <v>0.43167199999999895</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <v>1953</v>
       </c>
@@ -2370,7 +2370,7 @@
         <v>0.45278300000000371</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
         <v>1954</v>
       </c>
@@ -2391,7 +2391,7 @@
         <v>0.47389400000000137</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
         <v>1955</v>
       </c>
@@ -2412,7 +2412,7 @@
         <v>0.49500499999999903</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
         <v>1956</v>
       </c>
@@ -2433,7 +2433,7 @@
         <v>0.51611600000000379</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
         <v>1957</v>
       </c>
@@ -2454,7 +2454,7 @@
         <v>0.53722700000000145</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
         <v>1958</v>
       </c>
@@ -2475,7 +2475,7 @@
         <v>0.55833799999999911</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
         <v>1959</v>
       </c>
@@ -2496,7 +2496,7 @@
         <v>0.57999999999999996</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
         <v>1960</v>
       </c>
@@ -2516,7 +2516,7 @@
         <v>0.66028000000000731</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
         <v>1961</v>
       </c>
@@ -2536,7 +2536,7 @@
         <v>0.68742300000000967</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
         <v>1962</v>
       </c>
@@ -2556,7 +2556,7 @@
         <v>0.71456600000001202</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
         <v>1963</v>
       </c>
@@ -2576,7 +2576,7 @@
         <v>0.74170900000000728</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
         <v>1964</v>
       </c>
@@ -2596,7 +2596,7 @@
         <v>0.76885200000000964</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
         <v>1965</v>
       </c>
@@ -2616,7 +2616,7 @@
         <v>0.795995000000012</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
         <v>1966</v>
       </c>
@@ -2636,7 +2636,7 @@
         <v>0.82313800000000725</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
         <v>1967</v>
       </c>
@@ -2656,7 +2656,7 @@
         <v>0.85028100000000961</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
         <v>1968</v>
       </c>
@@ -2677,7 +2677,7 @@
         <v>0.85</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
         <v>1969</v>
       </c>
@@ -2699,7 +2699,7 @@
         <v>0.85</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
         <v>1970</v>
       </c>
@@ -2722,7 +2722,7 @@
         <v>0.85</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
         <v>1971</v>
       </c>
@@ -2746,7 +2746,7 @@
         <v>0.85</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
         <v>1972</v>
       </c>
@@ -2770,7 +2770,7 @@
         <v>0.85</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
         <v>1973</v>
       </c>
@@ -2794,7 +2794,7 @@
         <v>0.85</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
         <v>1974</v>
       </c>
@@ -2818,7 +2818,7 @@
         <v>0.85</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
         <v>1975</v>
       </c>
@@ -2842,7 +2842,7 @@
         <v>0.85</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
         <v>1976</v>
       </c>
@@ -2866,7 +2866,7 @@
         <v>0.85</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79" s="1">
         <v>1977</v>
       </c>
@@ -2890,7 +2890,7 @@
         <v>0.85</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
         <v>1978</v>
       </c>
@@ -2914,7 +2914,7 @@
         <v>0.85</v>
       </c>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81" s="1">
         <v>1979</v>
       </c>
@@ -2938,7 +2938,7 @@
         <v>0.85</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82" s="1">
         <v>1980</v>
       </c>
@@ -2962,7 +2962,7 @@
         <v>0.88</v>
       </c>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83" s="1">
         <v>1981</v>
       </c>
@@ -2986,7 +2986,7 @@
         <v>0.88</v>
       </c>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84" s="1">
         <v>1982</v>
       </c>
@@ -3010,7 +3010,7 @@
         <v>0.88</v>
       </c>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85" s="1">
         <v>1983</v>
       </c>
@@ -3034,7 +3034,7 @@
         <v>0.88</v>
       </c>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A86" s="1">
         <v>1984</v>
       </c>
@@ -3058,7 +3058,7 @@
         <v>0.88</v>
       </c>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A87" s="1">
         <v>1985</v>
       </c>
@@ -3082,7 +3082,7 @@
         <v>0.88</v>
       </c>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A88" s="1">
         <v>1986</v>
       </c>
@@ -3106,7 +3106,7 @@
         <v>0.88</v>
       </c>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89" s="1">
         <v>1987</v>
       </c>
@@ -3130,7 +3130,7 @@
         <v>0.88</v>
       </c>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A90" s="1">
         <v>1988</v>
       </c>
@@ -3154,7 +3154,7 @@
         <v>0.88</v>
       </c>
     </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A91" s="1">
         <v>1989</v>
       </c>
@@ -3178,7 +3178,7 @@
         <v>0.88</v>
       </c>
     </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A92" s="1">
         <v>1990</v>
       </c>
@@ -3202,7 +3202,7 @@
         <v>0.88</v>
       </c>
     </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A93" s="1">
         <v>1991</v>
       </c>
@@ -3226,7 +3226,7 @@
         <v>0.88</v>
       </c>
     </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A94" s="1">
         <v>1992</v>
       </c>
@@ -3250,7 +3250,7 @@
         <v>0.88</v>
       </c>
     </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A95" s="1">
         <v>1993</v>
       </c>
@@ -3274,7 +3274,7 @@
         <v>0.88</v>
       </c>
     </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A96" s="1">
         <v>1994</v>
       </c>
@@ -3298,7 +3298,7 @@
         <v>0.88</v>
       </c>
     </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A97" s="1">
         <v>1995</v>
       </c>
@@ -3320,7 +3320,7 @@
         <v>0.92</v>
       </c>
     </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A98" s="1">
         <v>1996</v>
       </c>
@@ -3343,7 +3343,7 @@
         <v>0.92</v>
       </c>
     </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A99" s="1">
         <v>1997</v>
       </c>
@@ -3366,7 +3366,7 @@
         <v>0.92</v>
       </c>
     </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A100" s="1">
         <v>1998</v>
       </c>
@@ -3389,7 +3389,7 @@
         <v>0.92</v>
       </c>
     </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A101" s="1">
         <v>1999</v>
       </c>
@@ -3412,7 +3412,7 @@
         <v>0.92</v>
       </c>
     </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A102" s="1">
         <v>2000</v>
       </c>
@@ -3435,7 +3435,7 @@
         <v>0.92</v>
       </c>
     </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A103" s="1">
         <v>2001</v>
       </c>
@@ -3458,7 +3458,7 @@
         <v>0.92</v>
       </c>
     </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A104" s="1">
         <v>2002</v>
       </c>
@@ -3481,7 +3481,7 @@
         <v>0.92</v>
       </c>
     </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A105" s="1">
         <v>2003</v>
       </c>
@@ -3504,7 +3504,7 @@
         <v>0.92</v>
       </c>
     </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A106" s="1">
         <v>2004</v>
       </c>
@@ -3527,7 +3527,7 @@
         <v>0.92</v>
       </c>
     </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A107" s="1">
         <v>2005</v>
       </c>
@@ -3550,7 +3550,7 @@
         <v>0.92</v>
       </c>
     </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A108" s="1">
         <v>2006</v>
       </c>
@@ -3573,7 +3573,7 @@
         <v>0.92</v>
       </c>
     </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A109" s="1">
         <v>2007</v>
       </c>
@@ -3596,7 +3596,7 @@
         <v>0.92</v>
       </c>
     </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A110" s="1">
         <v>2008</v>
       </c>
@@ -3618,7 +3618,7 @@
         <v>0.92</v>
       </c>
     </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A111" s="1">
         <v>2009</v>
       </c>
@@ -3640,7 +3640,7 @@
         <v>0.92</v>
       </c>
     </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A112" s="1">
         <v>2010</v>
       </c>
@@ -3660,7 +3660,7 @@
         <v>0.92</v>
       </c>
     </row>
-    <row r="113" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A113" s="1">
         <v>2011</v>
       </c>
@@ -3680,7 +3680,7 @@
         <v>0.92</v>
       </c>
     </row>
-    <row r="114" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A114" s="1">
         <v>2012</v>
       </c>
@@ -3700,7 +3700,7 @@
         <v>0.92</v>
       </c>
     </row>
-    <row r="115" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A115" s="1">
         <v>2013</v>
       </c>
@@ -3720,7 +3720,7 @@
         <v>0.92</v>
       </c>
     </row>
-    <row r="116" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A116" s="1">
         <v>2014</v>
       </c>
@@ -3740,7 +3740,7 @@
         <v>0.92</v>
       </c>
     </row>
-    <row r="117" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A117" s="1">
         <v>2015</v>
       </c>
@@ -3760,7 +3760,7 @@
         <v>0.92</v>
       </c>
     </row>
-    <row r="118" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A118" s="1">
         <v>2016</v>
       </c>
@@ -3780,7 +3780,7 @@
         <v>0.92</v>
       </c>
     </row>
-    <row r="119" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A119" s="1">
         <v>2017</v>
       </c>
@@ -3800,7 +3800,7 @@
         <v>0.92</v>
       </c>
     </row>
-    <row r="120" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A120" s="1">
         <v>2018</v>
       </c>
@@ -3820,7 +3820,7 @@
         <v>0.92</v>
       </c>
     </row>
-    <row r="121" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A121" s="1">
         <v>2019</v>
       </c>
@@ -3845,7 +3845,7 @@
         <v>0.92</v>
       </c>
     </row>
-    <row r="122" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A122" s="1">
         <v>2020</v>
       </c>
@@ -3870,7 +3870,7 @@
         <v>0.92</v>
       </c>
     </row>
-    <row r="123" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A123" s="1">
         <v>2021</v>
       </c>
@@ -3895,7 +3895,7 @@
         <v>0.92</v>
       </c>
     </row>
-    <row r="124" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A124" s="1">
         <v>2022</v>
       </c>
@@ -3920,7 +3920,7 @@
         <v>0.92</v>
       </c>
     </row>
-    <row r="125" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A125" s="1">
         <v>2023</v>
       </c>
@@ -3945,7 +3945,7 @@
         <v>0.92</v>
       </c>
     </row>
-    <row r="126" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A126" s="1">
         <v>2024</v>
       </c>
@@ -3970,7 +3970,7 @@
         <v>0.92</v>
       </c>
     </row>
-    <row r="127" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A127" s="1">
         <v>2025</v>
       </c>
@@ -3995,7 +3995,7 @@
         <v>0.92</v>
       </c>
     </row>
-    <row r="128" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A128" s="1">
         <v>2026</v>
       </c>
@@ -4020,7 +4020,7 @@
         <v>0.92</v>
       </c>
     </row>
-    <row r="129" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A129" s="1">
         <v>2027</v>
       </c>
@@ -4045,7 +4045,7 @@
         <v>0.92</v>
       </c>
     </row>
-    <row r="130" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A130" s="1">
         <v>2028</v>
       </c>
@@ -4070,7 +4070,7 @@
         <v>0.92</v>
       </c>
     </row>
-    <row r="131" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A131" s="1">
         <v>2029</v>
       </c>
@@ -4095,7 +4095,7 @@
         <v>0.92</v>
       </c>
     </row>
-    <row r="132" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A132" s="1">
         <v>2030</v>
       </c>
@@ -4120,7 +4120,7 @@
         <v>0.92</v>
       </c>
     </row>
-    <row r="133" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A133" s="1">
         <v>2031</v>
       </c>
@@ -4145,7 +4145,7 @@
         <v>0.92</v>
       </c>
     </row>
-    <row r="134" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A134" s="1">
         <v>2032</v>
       </c>
@@ -4170,7 +4170,7 @@
         <v>0.92</v>
       </c>
     </row>
-    <row r="135" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A135" s="1">
         <v>2033</v>
       </c>
@@ -4195,7 +4195,7 @@
         <v>0.92</v>
       </c>
     </row>
-    <row r="136" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A136" s="1">
         <v>2034</v>
       </c>
@@ -4220,7 +4220,7 @@
         <v>0.92</v>
       </c>
     </row>
-    <row r="137" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A137" s="1">
         <v>2035</v>
       </c>
@@ -4245,7 +4245,7 @@
         <v>0.92</v>
       </c>
     </row>
-    <row r="138" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A138" s="1">
         <v>2036</v>
       </c>
@@ -4270,7 +4270,7 @@
         <v>0.92</v>
       </c>
     </row>
-    <row r="139" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A139" s="1">
         <v>2037</v>
       </c>
@@ -4295,7 +4295,7 @@
         <v>0.92</v>
       </c>
     </row>
-    <row r="140" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A140" s="1">
         <v>2038</v>
       </c>
@@ -4320,7 +4320,7 @@
         <v>0.92</v>
       </c>
     </row>
-    <row r="141" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A141" s="1">
         <v>2039</v>
       </c>
@@ -4345,7 +4345,7 @@
         <v>0.92</v>
       </c>
     </row>
-    <row r="142" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A142" s="1">
         <v>2040</v>
       </c>
@@ -4370,7 +4370,7 @@
         <v>0.92</v>
       </c>
     </row>
-    <row r="143" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A143" s="1">
         <v>2041</v>
       </c>
@@ -4395,7 +4395,7 @@
         <v>0.92</v>
       </c>
     </row>
-    <row r="144" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A144" s="1">
         <v>2042</v>
       </c>
@@ -4420,7 +4420,7 @@
         <v>0.92</v>
       </c>
     </row>
-    <row r="145" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A145" s="1">
         <v>2043</v>
       </c>
@@ -4445,7 +4445,7 @@
         <v>0.92</v>
       </c>
     </row>
-    <row r="146" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A146" s="1">
         <v>2044</v>
       </c>
@@ -4470,7 +4470,7 @@
         <v>0.92</v>
       </c>
     </row>
-    <row r="147" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A147" s="1">
         <v>2045</v>
       </c>
@@ -4495,7 +4495,7 @@
         <v>0.92</v>
       </c>
     </row>
-    <row r="148" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A148" s="1">
         <v>2046</v>
       </c>
@@ -4520,7 +4520,7 @@
         <v>0.92</v>
       </c>
     </row>
-    <row r="149" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A149" s="1">
         <v>2047</v>
       </c>
@@ -4545,7 +4545,7 @@
         <v>0.92</v>
       </c>
     </row>
-    <row r="150" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A150" s="1">
         <v>2048</v>
       </c>
@@ -4570,7 +4570,7 @@
         <v>0.92</v>
       </c>
     </row>
-    <row r="151" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A151" s="1">
         <v>2049</v>
       </c>
@@ -4595,7 +4595,7 @@
         <v>0.92</v>
       </c>
     </row>
-    <row r="152" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A152" s="1">
         <v>2050</v>
       </c>
@@ -4622,847 +4622,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1FFAF0D-B3E5-43E3-9BF8-988D40819FB9}">
-  <dimension ref="A1:A151"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:A151"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1" s="13">
-        <v>0.45</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A2" s="13">
-        <v>0.45</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A3" s="13">
-        <v>0.45</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A4" s="13">
-        <v>0.45</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A5" s="13">
-        <v>0.45</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A6" s="13">
-        <v>0.45</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A7" s="13">
-        <v>0.45</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A8" s="13">
-        <v>0.45</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A9" s="13">
-        <v>0.45</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A10" s="13">
-        <v>0.45</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A11" s="13">
-        <v>0.45</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A12" s="13">
-        <v>0.45</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A13" s="13">
-        <v>0.45</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A14" s="13">
-        <v>0.45</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A15" s="13">
-        <v>0.45</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A16" s="13">
-        <v>0.45</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A17" s="13">
-        <v>0.45</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A18" s="13">
-        <v>0.45</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A19" s="13">
-        <v>0.45</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A20" s="13">
-        <v>0.45</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A21" s="13">
-        <v>0.45</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A22" s="13">
-        <v>0.45</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A23" s="13">
-        <v>0.45</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A24" s="13">
-        <v>0.45</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A25" s="13">
-        <v>0.45</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A26" s="13">
-        <v>0.45</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A27" s="13">
-        <v>0.45</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A28" s="13">
-        <v>0.45</v>
-      </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A29" s="13">
-        <v>0.45</v>
-      </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A30" s="13">
-        <v>0.45</v>
-      </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A31" s="13">
-        <v>0.45</v>
-      </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A32" s="13">
-        <v>0.45</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A33" s="13">
-        <v>0.45</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A34" s="13">
-        <v>0.45</v>
-      </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A35" s="13">
-        <v>0.45</v>
-      </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A36" s="13">
-        <v>0.45</v>
-      </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A37" s="13">
-        <v>0.45</v>
-      </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A38" s="13">
-        <v>0.45</v>
-      </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A39" s="13">
-        <v>0.45</v>
-      </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A40" s="13">
-        <v>0.45</v>
-      </c>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A41" s="13">
-        <v>0.45</v>
-      </c>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A42" s="13">
-        <v>0.45</v>
-      </c>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A43" s="13">
-        <v>0.45</v>
-      </c>
-    </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A44" s="13">
-        <v>0.45</v>
-      </c>
-    </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A45" s="13">
-        <v>0.45</v>
-      </c>
-    </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A46" s="13">
-        <v>0.45</v>
-      </c>
-    </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A47" s="13">
-        <v>0.45</v>
-      </c>
-    </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A48" s="13">
-        <v>0.45</v>
-      </c>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A49" s="13">
-        <v>0.45</v>
-      </c>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A50" s="13">
-        <v>0.45</v>
-      </c>
-    </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A51" s="13">
-        <v>0.45</v>
-      </c>
-    </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A52" s="13">
-        <v>0.45</v>
-      </c>
-    </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A53" s="13">
-        <v>0.45</v>
-      </c>
-    </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A54" s="13">
-        <v>0.45</v>
-      </c>
-    </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A55" s="13">
-        <v>0.45</v>
-      </c>
-    </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A56" s="13">
-        <v>0.45</v>
-      </c>
-    </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A57" s="13">
-        <v>0.45</v>
-      </c>
-    </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A58" s="13">
-        <v>0.45</v>
-      </c>
-    </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A59" s="13">
-        <v>0.45</v>
-      </c>
-    </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A60" s="13">
-        <v>0.45</v>
-      </c>
-    </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A61" s="13">
-        <v>0.45</v>
-      </c>
-    </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A62" s="13">
-        <v>0.45</v>
-      </c>
-    </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A63" s="13">
-        <v>0.45</v>
-      </c>
-    </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A64" s="13">
-        <v>0.45</v>
-      </c>
-    </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A65" s="13">
-        <v>0.45</v>
-      </c>
-    </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A66" s="13">
-        <v>0.45</v>
-      </c>
-    </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A67" s="13">
-        <v>0.45</v>
-      </c>
-    </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A68" s="13">
-        <v>0.45</v>
-      </c>
-    </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A69" s="13">
-        <v>0.45</v>
-      </c>
-    </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A70" s="13">
-        <v>0.45</v>
-      </c>
-    </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A71">
-        <f>0.92</f>
-        <v>0.92</v>
-      </c>
-    </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A72">
-        <f t="shared" ref="A72:A110" si="0">0.92</f>
-        <v>0.92</v>
-      </c>
-    </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A73">
-        <f t="shared" si="0"/>
-        <v>0.92</v>
-      </c>
-    </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A74">
-        <f t="shared" si="0"/>
-        <v>0.92</v>
-      </c>
-    </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A75">
-        <f t="shared" si="0"/>
-        <v>0.92</v>
-      </c>
-    </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A76">
-        <f t="shared" si="0"/>
-        <v>0.92</v>
-      </c>
-    </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A77">
-        <f t="shared" si="0"/>
-        <v>0.92</v>
-      </c>
-    </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A78">
-        <f t="shared" si="0"/>
-        <v>0.92</v>
-      </c>
-    </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A79">
-        <f t="shared" si="0"/>
-        <v>0.92</v>
-      </c>
-    </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A80">
-        <f t="shared" si="0"/>
-        <v>0.92</v>
-      </c>
-    </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A81">
-        <f t="shared" si="0"/>
-        <v>0.92</v>
-      </c>
-    </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A82">
-        <f t="shared" si="0"/>
-        <v>0.92</v>
-      </c>
-    </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A83">
-        <f t="shared" si="0"/>
-        <v>0.92</v>
-      </c>
-    </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A84">
-        <f t="shared" si="0"/>
-        <v>0.92</v>
-      </c>
-    </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A85">
-        <f t="shared" si="0"/>
-        <v>0.92</v>
-      </c>
-    </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A86">
-        <f t="shared" si="0"/>
-        <v>0.92</v>
-      </c>
-    </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A87">
-        <f t="shared" si="0"/>
-        <v>0.92</v>
-      </c>
-    </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A88">
-        <f t="shared" si="0"/>
-        <v>0.92</v>
-      </c>
-    </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A89">
-        <f t="shared" si="0"/>
-        <v>0.92</v>
-      </c>
-    </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A90">
-        <f t="shared" si="0"/>
-        <v>0.92</v>
-      </c>
-    </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A91">
-        <f t="shared" si="0"/>
-        <v>0.92</v>
-      </c>
-    </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A92">
-        <f t="shared" si="0"/>
-        <v>0.92</v>
-      </c>
-    </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A93">
-        <f t="shared" si="0"/>
-        <v>0.92</v>
-      </c>
-    </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A94">
-        <f t="shared" si="0"/>
-        <v>0.92</v>
-      </c>
-    </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A95">
-        <f t="shared" si="0"/>
-        <v>0.92</v>
-      </c>
-    </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A96">
-        <f t="shared" si="0"/>
-        <v>0.92</v>
-      </c>
-    </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A97">
-        <f t="shared" si="0"/>
-        <v>0.92</v>
-      </c>
-    </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A98">
-        <f t="shared" si="0"/>
-        <v>0.92</v>
-      </c>
-    </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A99">
-        <f t="shared" si="0"/>
-        <v>0.92</v>
-      </c>
-    </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A100">
-        <f t="shared" si="0"/>
-        <v>0.92</v>
-      </c>
-    </row>
-    <row r="101" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A101">
-        <f t="shared" si="0"/>
-        <v>0.92</v>
-      </c>
-    </row>
-    <row r="102" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A102">
-        <f t="shared" si="0"/>
-        <v>0.92</v>
-      </c>
-    </row>
-    <row r="103" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A103">
-        <f t="shared" si="0"/>
-        <v>0.92</v>
-      </c>
-    </row>
-    <row r="104" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A104">
-        <f t="shared" si="0"/>
-        <v>0.92</v>
-      </c>
-    </row>
-    <row r="105" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A105">
-        <f t="shared" si="0"/>
-        <v>0.92</v>
-      </c>
-    </row>
-    <row r="106" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A106">
-        <f t="shared" si="0"/>
-        <v>0.92</v>
-      </c>
-    </row>
-    <row r="107" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A107">
-        <f t="shared" si="0"/>
-        <v>0.92</v>
-      </c>
-    </row>
-    <row r="108" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A108">
-        <f t="shared" si="0"/>
-        <v>0.92</v>
-      </c>
-    </row>
-    <row r="109" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A109">
-        <f t="shared" si="0"/>
-        <v>0.92</v>
-      </c>
-    </row>
-    <row r="110" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A110">
-        <f t="shared" si="0"/>
-        <v>0.92</v>
-      </c>
-    </row>
-    <row r="111" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A111">
-        <v>0.99</v>
-      </c>
-    </row>
-    <row r="112" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A112">
-        <v>0.99</v>
-      </c>
-    </row>
-    <row r="113" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A113">
-        <v>0.99</v>
-      </c>
-    </row>
-    <row r="114" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A114">
-        <v>0.99</v>
-      </c>
-    </row>
-    <row r="115" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A115">
-        <v>0.99</v>
-      </c>
-    </row>
-    <row r="116" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A116">
-        <v>0.99</v>
-      </c>
-    </row>
-    <row r="117" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A117">
-        <v>0.99</v>
-      </c>
-    </row>
-    <row r="118" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A118">
-        <v>0.99</v>
-      </c>
-    </row>
-    <row r="119" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A119">
-        <v>0.99</v>
-      </c>
-    </row>
-    <row r="120" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A120" s="14">
-        <f>A119</f>
-        <v>0.99</v>
-      </c>
-    </row>
-    <row r="121" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A121" s="14">
-        <f t="shared" ref="A121:A151" si="1">A120</f>
-        <v>0.99</v>
-      </c>
-    </row>
-    <row r="122" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A122" s="14">
-        <f t="shared" si="1"/>
-        <v>0.99</v>
-      </c>
-    </row>
-    <row r="123" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A123" s="14">
-        <f t="shared" si="1"/>
-        <v>0.99</v>
-      </c>
-    </row>
-    <row r="124" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A124" s="14">
-        <f t="shared" si="1"/>
-        <v>0.99</v>
-      </c>
-    </row>
-    <row r="125" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A125" s="14">
-        <f t="shared" si="1"/>
-        <v>0.99</v>
-      </c>
-    </row>
-    <row r="126" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A126" s="14">
-        <f t="shared" si="1"/>
-        <v>0.99</v>
-      </c>
-    </row>
-    <row r="127" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A127" s="14">
-        <f t="shared" si="1"/>
-        <v>0.99</v>
-      </c>
-    </row>
-    <row r="128" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A128" s="14">
-        <f t="shared" si="1"/>
-        <v>0.99</v>
-      </c>
-    </row>
-    <row r="129" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A129" s="14">
-        <f t="shared" si="1"/>
-        <v>0.99</v>
-      </c>
-    </row>
-    <row r="130" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A130" s="14">
-        <f t="shared" si="1"/>
-        <v>0.99</v>
-      </c>
-    </row>
-    <row r="131" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A131" s="14">
-        <f t="shared" si="1"/>
-        <v>0.99</v>
-      </c>
-    </row>
-    <row r="132" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A132" s="14">
-        <f t="shared" si="1"/>
-        <v>0.99</v>
-      </c>
-    </row>
-    <row r="133" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A133" s="14">
-        <f t="shared" si="1"/>
-        <v>0.99</v>
-      </c>
-    </row>
-    <row r="134" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A134" s="14">
-        <f t="shared" si="1"/>
-        <v>0.99</v>
-      </c>
-    </row>
-    <row r="135" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A135" s="14">
-        <f t="shared" si="1"/>
-        <v>0.99</v>
-      </c>
-    </row>
-    <row r="136" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A136" s="14">
-        <f t="shared" si="1"/>
-        <v>0.99</v>
-      </c>
-    </row>
-    <row r="137" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A137" s="14">
-        <f t="shared" si="1"/>
-        <v>0.99</v>
-      </c>
-    </row>
-    <row r="138" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A138" s="14">
-        <f t="shared" si="1"/>
-        <v>0.99</v>
-      </c>
-    </row>
-    <row r="139" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A139" s="14">
-        <f t="shared" si="1"/>
-        <v>0.99</v>
-      </c>
-    </row>
-    <row r="140" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A140" s="14">
-        <f t="shared" si="1"/>
-        <v>0.99</v>
-      </c>
-    </row>
-    <row r="141" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A141" s="14">
-        <f t="shared" si="1"/>
-        <v>0.99</v>
-      </c>
-    </row>
-    <row r="142" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A142" s="14">
-        <f t="shared" si="1"/>
-        <v>0.99</v>
-      </c>
-    </row>
-    <row r="143" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A143" s="14">
-        <f t="shared" si="1"/>
-        <v>0.99</v>
-      </c>
-    </row>
-    <row r="144" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A144" s="14">
-        <f t="shared" si="1"/>
-        <v>0.99</v>
-      </c>
-    </row>
-    <row r="145" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A145" s="14">
-        <f t="shared" si="1"/>
-        <v>0.99</v>
-      </c>
-    </row>
-    <row r="146" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A146" s="14">
-        <f t="shared" si="1"/>
-        <v>0.99</v>
-      </c>
-    </row>
-    <row r="147" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A147" s="14">
-        <f t="shared" si="1"/>
-        <v>0.99</v>
-      </c>
-    </row>
-    <row r="148" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A148" s="14">
-        <f t="shared" si="1"/>
-        <v>0.99</v>
-      </c>
-    </row>
-    <row r="149" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A149" s="14">
-        <f t="shared" si="1"/>
-        <v>0.99</v>
-      </c>
-    </row>
-    <row r="150" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A150" s="14">
-        <f t="shared" si="1"/>
-        <v>0.99</v>
-      </c>
-    </row>
-    <row r="151" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A151" s="14">
-        <f t="shared" si="1"/>
-        <v>0.99</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>